<commit_message>
Ajout de la veille technologique
</commit_message>
<xml_diff>
--- a/assets/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (2).xlsx
+++ b/assets/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Documents\IMIE\PPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Documents\portfolio\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2676C8-AFF8-4DEC-8C71-5219730567AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2484F9-CC84-4CBD-AE89-8A52F1405967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -44,9 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Option :</t>
@@ -140,15 +136,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Du 4/12/21 au 20/12/21</t>
-  </si>
-  <si>
-    <t>Du 16/04/22 au 10/01/23</t>
-  </si>
-  <si>
-    <t>Du 01/06/22 au 15/06/22</t>
-  </si>
-  <si>
     <t>Du 12/12/22 au 15/12/22</t>
   </si>
   <si>
@@ -162,13 +149,61 @@
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Création du site web SPORT&amp;Co </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création de mon portfolio </t>
-  </si>
-  <si>
     <t>Mise à jour et déploiement de la nouvelle version d'un logiciel de pointage. Transfert de la base de données.</t>
+  </si>
+  <si>
+    <t>N° candidat : 02244094692</t>
+  </si>
+  <si>
+    <t>Création d'une application de gestion de consommation électrique en Java</t>
+  </si>
+  <si>
+    <t>Création d'une application de gestion de magazines en Java</t>
+  </si>
+  <si>
+    <t>Communication au sein du ministère sur l'utilisation de logiciel déployé</t>
+  </si>
+  <si>
+    <t>Du 18/12/22 au 20/12/22</t>
+  </si>
+  <si>
+    <t>Création d'une application de réservation de restaurant en Java</t>
+  </si>
+  <si>
+    <t>Du 23/01/23 au 26/01/23</t>
+  </si>
+  <si>
+    <t>Le 27/01/23</t>
+  </si>
+  <si>
+    <t>Création de mon portfolio en HTML, CSS et JavaScript</t>
+  </si>
+  <si>
+    <t>Création du site web SPORT&amp;Co en HTML et CSS</t>
+  </si>
+  <si>
+    <t>Présentation vidéo du métier d'apprenti en informatique publié sur le réseau intranet national</t>
+  </si>
+  <si>
+    <t>Du 27/01/23 au 30/01/23</t>
+  </si>
+  <si>
+    <t>Création d'un site de quiz en JavaScript avec NodeJS</t>
+  </si>
+  <si>
+    <t>Du 17/03/22 au 23/02/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Du 09/02/23 au </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création d'un profil Linkedin et d'une image professionnelle sur Internet </t>
+  </si>
+  <si>
+    <t>Du 09/11/22 au 15/11/22</t>
+  </si>
+  <si>
+    <t>Du 14/12/21 au 28/12/21</t>
   </si>
 </sst>
 </file>
@@ -653,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -728,75 +763,81 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1142,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1156,124 +1197,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="38"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="B6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1312,16 +1353,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="A8" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1360,22 +1401,22 @@
     </row>
     <row r="9" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>27</v>
+      <c r="E9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="G9" s="22"/>
-      <c r="H9" s="23" t="s">
-        <v>27</v>
+      <c r="H9" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
@@ -1415,20 +1456,20 @@
     </row>
     <row r="10" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>27</v>
+      <c r="G10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1468,24 +1509,24 @@
     </row>
     <row r="11" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>27</v>
+      <c r="E11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
@@ -1524,14 +1565,24 @@
       <c r="AQ11" s="24"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="F12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1569,14 +1620,22 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="F13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1614,14 +1673,22 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1659,14 +1726,20 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1704,7 +1777,6 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -1839,16 +1911,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="A19" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1885,68 +1957,74 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="49" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="27" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="B20" s="29">
+        <v>44440</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="F20" s="21"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="48"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="48"/>
-      <c r="AD20" s="48"/>
-      <c r="AE20" s="48"/>
-      <c r="AF20" s="48"/>
-      <c r="AG20" s="48"/>
-      <c r="AH20" s="48"/>
-      <c r="AI20" s="48"/>
-      <c r="AJ20" s="48"/>
-      <c r="AK20" s="48"/>
-      <c r="AL20" s="48"/>
-      <c r="AM20" s="48"/>
-      <c r="AN20" s="48"/>
-      <c r="AO20" s="48"/>
-      <c r="AP20" s="48"/>
-      <c r="AQ20" s="48"/>
+      <c r="H20" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="26"/>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="26"/>
+      <c r="AI20" s="26"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="26"/>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="26"/>
+      <c r="AO20" s="26"/>
+      <c r="AP20" s="26"/>
+      <c r="AQ20" s="26"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2209,16 +2287,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="A27" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2257,21 +2335,21 @@
     </row>
     <row r="28" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="22" t="s">
         <v>27</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
-      <c r="F28" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>27</v>
+      <c r="F28" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
@@ -2311,13 +2389,21 @@
       <c r="AQ28" s="24"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="H29" s="15"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -2356,14 +2442,20 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+      <c r="H30" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2673,11 +2765,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2685,6 +2772,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2695,6 +2787,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="949f60ab-cf46-4428-998c-a8263a1026bb" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04a24026-45de-4039-9a2a-7163b7f160de">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003161AC88D00B744AB848D3746258CD42" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5fb2091d76f3bee428fc8726e0901b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04a24026-45de-4039-9a2a-7163b7f160de" xmlns:ns3="949f60ab-cf46-4428-998c-a8263a1026bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6baa13dc209be22a675bb06314fb4ce" ns2:_="" ns3:_="">
     <xsd:import namespace="04a24026-45de-4039-9a2a-7163b7f160de"/>
@@ -2905,27 +3017,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D5361A-C5F4-4E8A-A4D3-3FC8A66372EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="949f60ab-cf46-4428-998c-a8263a1026bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="04a24026-45de-4039-9a2a-7163b7f160de"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="949f60ab-cf46-4428-998c-a8263a1026bb" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04a24026-45de-4039-9a2a-7163b7f160de">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C026E568-2EED-473E-BA81-EDFB8599479A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84F7394A-841A-42F5-B734-F824F6D3EA6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2942,23 +3059,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C026E568-2EED-473E-BA81-EDFB8599479A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D5361A-C5F4-4E8A-A4D3-3FC8A66372EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="949f60ab-cf46-4428-998c-a8263a1026bb"/>
-    <ds:schemaRef ds:uri="04a24026-45de-4039-9a2a-7163b7f160de"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New style and content updated
</commit_message>
<xml_diff>
--- a/assets/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (2).xlsx
+++ b/assets/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Documents\portfolio\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2484F9-CC84-4CBD-AE89-8A52F1405967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2974E-896A-4781-A600-B6C3651011A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
-  </si>
-  <si>
-    <t>SESSION 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
@@ -145,58 +142,33 @@
     <t>Du 03/01/22 au 07/01/22</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisation d'un jeu de Memory en JavaScript
- </t>
-  </si>
-  <si>
     <t>Mise à jour et déploiement de la nouvelle version d'un logiciel de pointage. Transfert de la base de données.</t>
   </si>
   <si>
     <t>N° candidat : 02244094692</t>
   </si>
   <si>
-    <t>Création d'une application de gestion de consommation électrique en Java</t>
-  </si>
-  <si>
-    <t>Création d'une application de gestion de magazines en Java</t>
-  </si>
-  <si>
     <t>Communication au sein du ministère sur l'utilisation de logiciel déployé</t>
   </si>
   <si>
     <t>Du 18/12/22 au 20/12/22</t>
   </si>
   <si>
-    <t>Création d'une application de réservation de restaurant en Java</t>
-  </si>
-  <si>
     <t>Du 23/01/23 au 26/01/23</t>
   </si>
   <si>
     <t>Le 27/01/23</t>
   </si>
   <si>
-    <t>Création de mon portfolio en HTML, CSS et JavaScript</t>
-  </si>
-  <si>
-    <t>Création du site web SPORT&amp;Co en HTML et CSS</t>
-  </si>
-  <si>
     <t>Présentation vidéo du métier d'apprenti en informatique publié sur le réseau intranet national</t>
   </si>
   <si>
     <t>Du 27/01/23 au 30/01/23</t>
   </si>
   <si>
-    <t>Création d'un site de quiz en JavaScript avec NodeJS</t>
-  </si>
-  <si>
     <t>Du 17/03/22 au 23/02/23</t>
   </si>
   <si>
-    <t xml:space="preserve">Du 09/02/23 au </t>
-  </si>
-  <si>
     <t xml:space="preserve">Création d'un profil Linkedin et d'une image professionnelle sur Internet </t>
   </si>
   <si>
@@ -204,6 +176,46 @@
   </si>
   <si>
     <t>Du 14/12/21 au 28/12/21</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
+  </si>
+  <si>
+    <t>Recensement du patrimoine informatique du site, et proposition d'amélioration de ce dernier conformément au budget imposé.</t>
+  </si>
+  <si>
+    <t>Du 11/07/22 au 19/07/22</t>
+  </si>
+  <si>
+    <t>Création d'un site de quiz en JavaScript avec NodeJS (code source)</t>
+  </si>
+  <si>
+    <t>Création d'une application de réservation de restaurant en Java (code source)</t>
+  </si>
+  <si>
+    <t>Création d'une application de gestion de magazines en Java (code source)</t>
+  </si>
+  <si>
+    <t>Création d'une application de gestion de consommation électrique en Java avec test unitaires (code source)</t>
+  </si>
+  <si>
+    <t>Création de mon portfolio en HTML, CSS et JavaScript       https://mathis-laversin.site (code source)</t>
+  </si>
+  <si>
+    <t>Réalisation d'un jeu de Memory en JavaScript
+ (code source)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du site web SPORT&amp;Co en HTML et CSS </t>
+  </si>
+  <si>
+    <t>Création d'un site web en React et Strapi</t>
+  </si>
+  <si>
+    <t>Du 09/02/23 au 23/02/23</t>
+  </si>
+  <si>
+    <t>Du 21/03/23 au 07/04/23</t>
   </si>
 </sst>
 </file>
@@ -773,9 +785,48 @@
     <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -798,45 +849,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1183,8 +1195,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1197,124 +1209,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
+      <c r="A3" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="51"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="A4" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="51"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="B6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1353,16 +1365,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
+      <c r="A8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1401,22 +1413,22 @@
     </row>
     <row r="9" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
@@ -1456,20 +1468,20 @@
     </row>
     <row r="10" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1509,24 +1521,24 @@
     </row>
     <row r="11" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
@@ -1566,22 +1578,22 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1621,20 +1633,20 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
@@ -1674,20 +1686,20 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1730,7 +1742,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1738,7 +1750,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1777,13 +1789,26 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="E16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>25</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1911,16 +1936,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
+      <c r="A19" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1959,7 +1984,7 @@
     </row>
     <row r="20" spans="1:43" s="27" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B20" s="29">
         <v>44440</v>
@@ -1970,7 +1995,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="22"/>
       <c r="H20" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="26"/>
@@ -2010,20 +2035,20 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2062,12 +2087,20 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22"/>
@@ -2287,16 +2320,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="46"/>
+      <c r="A27" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2335,21 +2368,21 @@
     </row>
     <row r="28" spans="1:43" s="25" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
@@ -2390,19 +2423,19 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H29" s="15"/>
       <c r="I29"/>
@@ -2443,18 +2476,18 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -2765,6 +2798,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2772,11 +2810,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2787,26 +2820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="949f60ab-cf46-4428-998c-a8263a1026bb" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04a24026-45de-4039-9a2a-7163b7f160de">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003161AC88D00B744AB848D3746258CD42" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5fb2091d76f3bee428fc8726e0901b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04a24026-45de-4039-9a2a-7163b7f160de" xmlns:ns3="949f60ab-cf46-4428-998c-a8263a1026bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6baa13dc209be22a675bb06314fb4ce" ns2:_="" ns3:_="">
     <xsd:import namespace="04a24026-45de-4039-9a2a-7163b7f160de"/>
@@ -3017,32 +3030,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D5361A-C5F4-4E8A-A4D3-3FC8A66372EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="949f60ab-cf46-4428-998c-a8263a1026bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="04a24026-45de-4039-9a2a-7163b7f160de"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C026E568-2EED-473E-BA81-EDFB8599479A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="949f60ab-cf46-4428-998c-a8263a1026bb" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04a24026-45de-4039-9a2a-7163b7f160de">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84F7394A-841A-42F5-B734-F824F6D3EA6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3059,4 +3067,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C026E568-2EED-473E-BA81-EDFB8599479A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D5361A-C5F4-4E8A-A4D3-3FC8A66372EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="949f60ab-cf46-4428-998c-a8263a1026bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="04a24026-45de-4039-9a2a-7163b7f160de"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>